<commit_message>
Defined input of cutadapt; Mageck count is now working as expected
</commit_message>
<xml_diff>
--- a/test-data/DataSheet.xlsx
+++ b/test-data/DataSheet.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test-data_demo2_test.fastq.gz</t>
+          <t>CTRL_R1_T1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>test-data_demo2_test1.fastq.gz</t>
+          <t>L1_R1_T1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>